<commit_message>
Fixed issue with minutes if ionterval more than a day
</commit_message>
<xml_diff>
--- a/public/templates/review-audit-template.xlsx
+++ b/public/templates/review-audit-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Act/onefile-tools/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DADF70-DEA3-7B4D-925C-4FD9D29FE9DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE40EF56-42AE-9749-9E36-1B5166A87D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8000" yWindow="2920" windowWidth="29340" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -295,7 +295,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -318,11 +318,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -333,16 +333,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -14013,20 +14003,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AF2:AF250">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF2:AF250">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K250">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>